<commit_message>
tested model in initial phase
</commit_message>
<xml_diff>
--- a/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
+++ b/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dthoms\Documents\Training\Coursera\Johns.Hopkins.Data.Science.Specialization\NLP.project\R.Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEDEB52-A2CE-4DEB-AE99-E06027056167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27919D88-D820-4866-88E6-A80A4D888ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98F435A4-3A33-4075-849B-0D63A5FCEF36}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Version</t>
   </si>
@@ -54,10 +54,6 @@
   <si>
     <t>[1] "Ohhhhh #PointBreak is on tomorrow. Love that film and haven't seen it in quite some"
 [1] "time"</t>
-  </si>
-  <si>
-    <t>[1] "Well I'm pretty sure my granny has some old bagpipes in her garage I'll dust them off and be on my"
-[1] "way starting"</t>
   </si>
   <si>
     <t>PASS</t>
@@ -122,9 +118,6 @@
 predit - less than 1 min</t>
   </si>
   <si>
-    <t>[1] "Hey sunshine, can you follow me and make me the"</t>
-  </si>
-  <si>
     <t>[1] "opportunity to"</t>
   </si>
   <si>
@@ -267,6 +260,62 @@
   </si>
   <si>
     <t>next step, store whole data</t>
+  </si>
+  <si>
+    <t>close to 100%</t>
+  </si>
+  <si>
+    <t>unigram-bigram - 3, trigram - 2, others  -1 removed</t>
+  </si>
+  <si>
+    <t>the - problem, popular stop word</t>
+  </si>
+  <si>
+    <t>fail - many more have higher chance</t>
+  </si>
+  <si>
+    <t>end (higher level 4 gram found, it quit</t>
+  </si>
+  <si>
+    <t>brother - didn't go deep enough</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - didn't go low enouch</t>
+  </si>
+  <si>
+    <t>must be doing - didn't go low enough</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>yes, removed as final answers</t>
+  </si>
+  <si>
+    <t>all opetions taken</t>
+  </si>
+  <si>
+    <t>[1] "Well I'm pretty sure my granny has some old bagpipes in her garage I'll dust them off and be on my"
+[1] "way"</t>
+  </si>
+  <si>
+    <t>[1] "Hey sunshine, can you follow me and make me the"
+[1] happiest</t>
+  </si>
+  <si>
+    <t>fail - best</t>
+  </si>
+  <si>
+    <t>fail - end</t>
+  </si>
+  <si>
+    <t>fail - brother</t>
+  </si>
+  <si>
+    <t>fail - day</t>
+  </si>
+  <si>
+    <t>fail - able</t>
   </si>
 </sst>
 </file>
@@ -658,13 +707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AA7307-9F72-465A-9E11-419EBFDD9B16}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="N11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +727,8 @@
     <col min="20" max="20" width="44.5546875" customWidth="1"/>
     <col min="21" max="21" width="37.6640625" customWidth="1"/>
     <col min="22" max="22" width="35.6640625" customWidth="1"/>
-    <col min="24" max="29" width="16.88671875" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" customWidth="1"/>
+    <col min="25" max="29" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -691,22 +741,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
@@ -715,31 +765,31 @@
         <v>3</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>12</v>
-      </c>
-      <c r="S2" t="s">
-        <v>13</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>5</v>
@@ -748,28 +798,28 @@
         <v>6</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="X2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="AA2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
@@ -795,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q3">
         <v>3</v>
@@ -808,13 +858,13 @@
         <v>0.3</v>
       </c>
       <c r="T3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
@@ -846,10 +896,10 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S4" t="e">
         <f t="shared" ref="S4:S7" si="0">Q4/(Q4+R4)</f>
@@ -876,13 +926,13 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" t="s">
         <v>19</v>
-      </c>
-      <c r="N5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" t="s">
-        <v>20</v>
       </c>
       <c r="S5" t="e">
         <f t="shared" si="0"/>
@@ -909,13 +959,13 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" t="s">
         <v>21</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" t="s">
-        <v>22</v>
       </c>
       <c r="S6" t="e">
         <f t="shared" si="0"/>
@@ -930,7 +980,7 @@
         <v>4.4400000000000002E-2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>200438</v>
@@ -951,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q7">
         <v>3</v>
@@ -967,34 +1017,34 @@
         <v>0.3</v>
       </c>
       <c r="T7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA7" s="5" t="s">
+      <c r="AB7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AB7" s="5" t="s">
+      <c r="AC7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="AC7" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
@@ -1005,13 +1055,13 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2">
         <v>800851</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1026,40 +1076,40 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V8" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC8" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="V8" t="s">
-        <v>42</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
@@ -1088,40 +1138,40 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="V9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB9" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="AC9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="86.4" x14ac:dyDescent="0.3">
@@ -1132,7 +1182,7 @@
         <v>0.13343869999999999</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>1204675</v>
@@ -1153,56 +1203,56 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T10" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U10" t="s">
-        <v>43</v>
-      </c>
-      <c r="V10" t="s">
-        <v>42</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="X10" s="3" t="s">
+      <c r="Z10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Y10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z10" s="5" t="s">
+      <c r="AA10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AA10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB10" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="AC10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
@@ -1213,7 +1263,7 @@
         <v>0.13343869999999999</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1228,16 +1278,16 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
@@ -1266,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q15">
         <v>3</v>
@@ -1278,39 +1328,163 @@
         <v>10</v>
       </c>
       <c r="T15" t="s">
+        <v>68</v>
+      </c>
+      <c r="U15" t="s">
+        <v>68</v>
+      </c>
+      <c r="V15" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" t="s">
+        <v>57</v>
+      </c>
+      <c r="X15" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y15" t="s">
         <v>70</v>
       </c>
-      <c r="U15" t="s">
-        <v>70</v>
-      </c>
-      <c r="V15" t="s">
-        <v>70</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="Z15" t="s">
         <v>71</v>
       </c>
-      <c r="X15" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>72</v>
       </c>
-      <c r="Z15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>74</v>
-      </c>
       <c r="AB15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" t="s">
         <v>75</v>
+      </c>
+      <c r="N17" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <v>0.5</v>
+      </c>
+      <c r="T17" t="s">
+        <v>68</v>
+      </c>
+      <c r="U17" t="s">
+        <v>68</v>
+      </c>
+      <c r="V17" t="s">
+        <v>68</v>
+      </c>
+      <c r="W17" t="s">
+        <v>68</v>
+      </c>
+      <c r="X17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>0.5</v>
+      </c>
+      <c r="T18" t="s">
+        <v>68</v>
+      </c>
+      <c r="U18" t="s">
+        <v>68</v>
+      </c>
+      <c r="V18" t="s">
+        <v>68</v>
+      </c>
+      <c r="W18" t="s">
+        <v>68</v>
+      </c>
+      <c r="X18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try kneser ney model
</commit_message>
<xml_diff>
--- a/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
+++ b/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dthoms\Documents\Training\Coursera\Johns.Hopkins.Data.Science.Specialization\NLP.project\R.Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D905301-B361-4934-A641-00477B52CE6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49466DB6-2B62-48BE-95CF-C83BFB3CC51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{98F435A4-3A33-4075-849B-0D63A5FCEF36}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
   <si>
     <t>Version</t>
   </si>
@@ -377,9 +377,6 @@
     <t>fail - morning</t>
   </si>
   <si>
-    <t>pass - stress</t>
-  </si>
-  <si>
     <t>fail - look</t>
   </si>
   <si>
@@ -393,6 +390,30 @@
   </si>
   <si>
     <t>pass - outside</t>
+  </si>
+  <si>
+    <t>extra corpus</t>
+  </si>
+  <si>
+    <t>fixed capital issues with sentence</t>
+  </si>
+  <si>
+    <t>top - like, options - die</t>
+  </si>
+  <si>
+    <t>top - orphan, options - spiritual</t>
+  </si>
+  <si>
+    <t>fail - stress</t>
+  </si>
+  <si>
+    <t>matter</t>
+  </si>
+  <si>
+    <t>pass - top - case, options hand</t>
+  </si>
+  <si>
+    <t>pass - top - basketball, options - outside</t>
   </si>
 </sst>
 </file>
@@ -1584,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0E42B5-E1D9-4386-9AE6-E588BF013FBD}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,30 +1754,66 @@
         <v>110</v>
       </c>
       <c r="W2" t="s">
+        <v>120</v>
+      </c>
+      <c r="X2" t="s">
         <v>111</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>112</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>113</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>114</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="AC2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="O3" t="s">
+        <v>117</v>
+      </c>
+      <c r="T3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U3" t="s">
+        <v>119</v>
+      </c>
+      <c r="V3" t="s">
+        <v>110</v>
+      </c>
+      <c r="W3" t="s">
+        <v>120</v>
+      </c>
+      <c r="X3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>

</xml_diff>

<commit_message>
optimized model for speed and size
</commit_message>
<xml_diff>
--- a/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
+++ b/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dthoms\Documents\Training\Coursera\Johns.Hopkins.Data.Science.Specialization\NLP.project\R.Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49466DB6-2B62-48BE-95CF-C83BFB3CC51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ABEE8C-0B04-41CF-A00A-B204B8A62F85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{98F435A4-3A33-4075-849B-0D63A5FCEF36}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{98F435A4-3A33-4075-849B-0D63A5FCEF36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="R. benchmark" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>Version</t>
   </si>
@@ -414,6 +415,26 @@
   </si>
   <si>
     <t>pass - top - basketball, options - outside</t>
+  </si>
+  <si>
+    <t>unigram</t>
+  </si>
+  <si>
+    <t>top 500</t>
+  </si>
+  <si>
+    <t>numer per root</t>
+  </si>
+  <si>
+    <t>Overall top-3 score:     14.68 %
+Overall top-1 precision: 10.66 %
+Overall top-3 precision: 17.72 %
+Average runtime:         910.16 msec
+Number of predictions:   448
+Total memory used:       2319.75 MB</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0E42B5-E1D9-4386-9AE6-E588BF013FBD}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
@@ -1846,4 +1867,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D4DBA7-6546-4D63-A273-2C8CB4209694}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>0.15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>0.4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaning up final finish
</commit_message>
<xml_diff>
--- a/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
+++ b/Johns.Hopkins.Data.Science.Specialization/NLP.project/R.Project/Model-improvement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dthoms\Documents\Training\Coursera\Johns.Hopkins.Data.Science.Specialization\NLP.project\R.Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A073C8-CD8C-49A4-AC98-4812137D76CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF7A840-D04C-4DDE-B1FA-CA8C7E355D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{98F435A4-3A33-4075-849B-0D63A5FCEF36}"/>
   </bookViews>
@@ -564,14 +564,6 @@
     <t>full</t>
   </si>
   <si>
-    <t>Overall top-3 score:     16.11 %
-Overall top-1 precision: 12.21 %
-Overall top-3 precision: 19.54 %
-Average runtime:         51.49 msec
-Number of predictions:   28464
-Total memory used:       1702.27 MB</t>
-  </si>
-  <si>
     <t>frequency of words 12 and up, ignore size as extra items in env</t>
   </si>
   <si>
@@ -584,6 +576,14 @@
   </si>
   <si>
     <t>removed stop words, very poor performance, need them</t>
+  </si>
+  <si>
+    <t>Overall top-3 score:     16.11 %
+Overall top-1 precision: 12.21 %
+Overall top-3 precision: 19.54 %
+Average runtime:         51.49 msec
+Number of predictions:   28464
+Total memory used:       84.84 MB</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -645,12 +645,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -671,6 +686,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2026,7 +2044,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,7 +2319,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -2318,10 +2336,10 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -2334,11 +2352,11 @@
       <c r="D15" t="s">
         <v>135</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" t="s">
         <v>153</v>
-      </c>
-      <c r="F15" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -2355,10 +2373,10 @@
         <v>135</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" t="s">
         <v>155</v>
-      </c>
-      <c r="F16" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>